<commit_message>
Began to refactor + add external factors to evaluations
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/new Max matrix.xlsx
+++ b/src/main/resources/excel/new Max matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikita/Desktop/Аспирантура/Макс/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikita/IdeaProjects/derivative_toy/src/main/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9165B519-BF28-6E49-A586-A06E83F1942A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361A2380-C761-2E4B-9CD9-6A948F298A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{96483E0F-6F8A-7647-8A7C-E9C205EC2003}"/>
   </bookViews>
@@ -408,7 +408,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,31 +422,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -505,21 +493,20 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -897,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE1A6C4-C313-614E-8C51-B298D5149A54}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="42" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,33 +918,33 @@
   <sheetData>
     <row r="1" spans="1:26" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="21" t="s">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
     </row>
     <row r="2" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
@@ -1020,16 +1007,16 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16">
-        <v>0</v>
-      </c>
-      <c r="C3" s="17">
+      <c r="B3" s="19">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19">
         <v>1</v>
       </c>
       <c r="D3" s="14">
         <v>1</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="19">
         <v>0</v>
       </c>
       <c r="F3" s="14">
@@ -1077,7 +1064,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="20">
         <v>1</v>
       </c>
       <c r="C4" s="15">
@@ -1191,7 +1178,7 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <v>-1</v>
       </c>
       <c r="C6" s="15">

</xml_diff>